<commit_message>
updated with additional graph and database text file
</commit_message>
<xml_diff>
--- a/HW4/data.xlsx
+++ b/HW4/data.xlsx
@@ -286,11 +286,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2144304904"/>
-        <c:axId val="2143625384"/>
+        <c:axId val="2120878232"/>
+        <c:axId val="2120881176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2144304904"/>
+        <c:axId val="2120878232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,7 +300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143625384"/>
+        <c:crossAx val="2120881176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -308,7 +308,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143625384"/>
+        <c:axId val="2120881176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -319,7 +319,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144304904"/>
+        <c:crossAx val="2120878232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -429,11 +429,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2109698104"/>
-        <c:axId val="-2109448408"/>
+        <c:axId val="2120943512"/>
+        <c:axId val="2120946456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2109698104"/>
+        <c:axId val="2120943512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,7 +443,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109448408"/>
+        <c:crossAx val="2120946456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -451,7 +451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2109448408"/>
+        <c:axId val="2120946456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -462,7 +462,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109698104"/>
+        <c:crossAx val="2120943512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -572,11 +572,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2110850984"/>
-        <c:axId val="-2110848040"/>
+        <c:axId val="2120971352"/>
+        <c:axId val="2120974296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2110850984"/>
+        <c:axId val="2120971352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -586,7 +586,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110848040"/>
+        <c:crossAx val="2120974296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -594,7 +594,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110848040"/>
+        <c:axId val="2120974296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -605,7 +605,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110850984"/>
+        <c:crossAx val="2120971352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -715,11 +715,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2139059928"/>
-        <c:axId val="2139062872"/>
+        <c:axId val="2120999128"/>
+        <c:axId val="2121002072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2139059928"/>
+        <c:axId val="2120999128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -729,7 +729,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139062872"/>
+        <c:crossAx val="2121002072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -737,7 +737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2139062872"/>
+        <c:axId val="2121002072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,11 +748,356 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139059928"/>
+        <c:crossAx val="2120999128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Runtime</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Double</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.002442</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.013485</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.021503</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.039024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.060301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ten</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.004794</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01172</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.024437</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.040911</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.06002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>One</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.011577</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.036026</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.079854</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.133131</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.199275</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Linked</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.005847</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.016696</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.033015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.055949</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.083879</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2132751448"/>
+        <c:axId val="2132754536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2132751448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2132754536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2132754536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2132751448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -987,10 +1332,49 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t> increase.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Double is fastest, then ten %, then linked, then +1.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1321,7 +1705,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>